<commit_message>
merge HCP's version with CYQ's
</commit_message>
<xml_diff>
--- a/Education & Occupation recode_ver2.xlsx
+++ b/Education & Occupation recode_ver2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/y_cai2_uu_nl/Documents/4_2_2_Formal reproduction/From github 230221/Flexibility_SES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="500" documentId="11_C0134E8D79783741A1729EDB151F7E74109EE093" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{818EDF57-E462-4A7B-9BC4-3B173717DF4D}"/>
+  <xr:revisionPtr revIDLastSave="502" documentId="11_C0134E8D79783741A1729EDB151F7E74109EE093" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D5E4B0A-E5AC-4618-BFF9-DD26C83C34B1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11250" yWindow="5235" windowWidth="6405" windowHeight="3345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="392">
   <si>
     <t>CFPS egp</t>
   </si>
@@ -1351,6 +1351,27 @@
   </si>
   <si>
     <t>post-graduate</t>
+  </si>
+  <si>
+    <t>Salzwedel, 2016</t>
+  </si>
+  <si>
+    <t>3 = some high school</t>
+  </si>
+  <si>
+    <t>4 = high school</t>
+  </si>
+  <si>
+    <t>5 = trade/bus</t>
+  </si>
+  <si>
+    <t>6 = some college</t>
+  </si>
+  <si>
+    <t>7 = college</t>
+  </si>
+  <si>
+    <t>8 = post-grad</t>
   </si>
 </sst>
 </file>
@@ -1938,7 +1959,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2054,8 +2075,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2063,23 +2084,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2090,26 +2102,47 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2117,29 +2150,20 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2734,11 +2758,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG1001"/>
+  <dimension ref="A1:AH1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA71" sqref="AA71"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH53" sqref="AH53:AH71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1"/>
@@ -2804,34 +2828,34 @@
       <c r="A2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="71" t="s">
         <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="51" t="s">
         <v>175</v>
       </c>
       <c r="J2" s="3">
         <v>0</v>
       </c>
-      <c r="K2" s="49" t="s">
+      <c r="K2" s="54" t="s">
         <v>200</v>
       </c>
       <c r="L2" s="46" t="s">
@@ -2851,23 +2875,23 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="54" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
       <c r="J3" s="47">
         <v>6</v>
       </c>
-      <c r="K3" s="58"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="47"/>
       <c r="M3" s="47"/>
       <c r="N3" s="46" t="s">
@@ -2877,17 +2901,17 @@
       <c r="P3" s="47"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
       <c r="J4" s="47"/>
-      <c r="K4" s="58"/>
+      <c r="K4" s="55"/>
       <c r="L4" s="47"/>
       <c r="M4" s="47"/>
       <c r="N4" s="46"/>
@@ -2895,25 +2919,25 @@
       <c r="P4" s="47"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54" t="s">
+      <c r="B5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="H5" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="54"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="47">
         <v>9</v>
       </c>
-      <c r="K5" s="49" t="s">
+      <c r="K5" s="54" t="s">
         <v>201</v>
       </c>
       <c r="L5" s="46" t="s">
@@ -2927,17 +2951,17 @@
       <c r="P5" s="47"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="47"/>
-      <c r="K6" s="49"/>
+      <c r="K6" s="54"/>
       <c r="L6" s="47"/>
       <c r="M6" s="47"/>
       <c r="N6" s="46"/>
@@ -2945,19 +2969,19 @@
       <c r="P6" s="47"/>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1">
-      <c r="A7" s="54"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
       <c r="H7" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="54"/>
+      <c r="I7" s="51"/>
       <c r="J7" s="47"/>
-      <c r="K7" s="49"/>
+      <c r="K7" s="54"/>
       <c r="L7" s="47"/>
       <c r="M7" s="47"/>
       <c r="N7" s="46"/>
@@ -2965,35 +2989,35 @@
       <c r="P7" s="47"/>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54" t="s">
+      <c r="E8" s="51"/>
+      <c r="F8" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="J8" s="48">
+      <c r="J8" s="50">
         <v>12</v>
       </c>
-      <c r="K8" s="49" t="s">
+      <c r="K8" s="54" t="s">
         <v>202</v>
       </c>
       <c r="L8" s="46" t="s">
@@ -3005,17 +3029,17 @@
       <c r="P8" s="47"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1">
-      <c r="A9" s="54"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="58"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="46"/>
       <c r="M9" s="47"/>
       <c r="N9" s="46"/>
@@ -3023,17 +3047,17 @@
       <c r="P9" s="47"/>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1">
-      <c r="A10" s="54"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="58"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="55"/>
       <c r="L10" s="46"/>
       <c r="M10" s="47"/>
       <c r="N10" s="46"/>
@@ -3041,17 +3065,17 @@
       <c r="P10" s="47"/>
     </row>
     <row r="11" spans="1:16" ht="15" customHeight="1">
-      <c r="A11" s="54"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="58"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="55"/>
       <c r="L11" s="46"/>
       <c r="M11" s="47"/>
       <c r="N11" s="46"/>
@@ -3059,37 +3083,37 @@
       <c r="P11" s="47"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="51">
         <v>2</v>
       </c>
-      <c r="F12" s="54" t="s">
+      <c r="F12" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="G12" s="54" t="s">
+      <c r="G12" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="54" t="s">
+      <c r="H12" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="I12" s="55" t="s">
+      <c r="I12" s="52" t="s">
         <v>169</v>
       </c>
       <c r="J12" s="47">
         <v>15</v>
       </c>
-      <c r="K12" s="49" t="s">
+      <c r="K12" s="54" t="s">
         <v>203</v>
       </c>
       <c r="L12" s="46" t="s">
@@ -3109,15 +3133,15 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A13" s="54"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="55"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="52"/>
       <c r="J13" s="47"/>
       <c r="K13" s="47"/>
       <c r="L13" s="47"/>
@@ -3127,29 +3151,29 @@
       <c r="P13" s="47"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="55" t="s">
+      <c r="D14" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="54"/>
-      <c r="F14" s="55" t="s">
+      <c r="E14" s="51"/>
+      <c r="F14" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="55" t="s">
+      <c r="G14" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="H14" s="55" t="s">
+      <c r="H14" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="I14" s="55" t="s">
+      <c r="I14" s="52" t="s">
         <v>170</v>
       </c>
       <c r="J14" s="47">
@@ -3165,15 +3189,15 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A15" s="54"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
       <c r="J15" s="47"/>
       <c r="K15" s="47"/>
       <c r="L15" s="47"/>
@@ -3183,15 +3207,15 @@
       <c r="P15" s="47"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A16" s="54"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
       <c r="J16" s="47"/>
       <c r="K16" s="47"/>
       <c r="L16" s="47"/>
@@ -3200,36 +3224,36 @@
       <c r="O16" s="47"/>
       <c r="P16" s="47"/>
     </row>
-    <row r="17" spans="1:28" ht="15.75" customHeight="1">
+    <row r="17" spans="1:29" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="51" t="s">
         <v>132</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="54"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="3" t="s">
         <v>100</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H17" s="54" t="s">
+      <c r="H17" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="I17" s="54" t="s">
+      <c r="I17" s="51" t="s">
         <v>171</v>
       </c>
       <c r="J17" s="3">
         <v>17</v>
       </c>
-      <c r="K17" s="49" t="s">
+      <c r="K17" s="54" t="s">
         <v>204</v>
       </c>
       <c r="L17" s="46" t="s">
@@ -3242,44 +3266,44 @@
         <v>291</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="15.75" customHeight="1">
+    <row r="18" spans="1:29" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="54"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
       <c r="F18" s="3" t="s">
         <v>101</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
       <c r="J18" s="3">
         <v>18</v>
       </c>
-      <c r="K18" s="49"/>
+      <c r="K18" s="54"/>
       <c r="L18" s="47"/>
       <c r="M18" s="47"/>
       <c r="N18" s="46"/>
       <c r="O18" s="47"/>
       <c r="P18" s="47"/>
     </row>
-    <row r="19" spans="1:28" ht="15.75" customHeight="1">
+    <row r="19" spans="1:29" ht="15.75" customHeight="1">
       <c r="N19" s="28"/>
     </row>
-    <row r="20" spans="1:28" ht="15.75" customHeight="1">
+    <row r="20" spans="1:29" ht="15.75" customHeight="1">
       <c r="N20" s="28"/>
     </row>
-    <row r="21" spans="1:28" ht="15.75" customHeight="1">
+    <row r="21" spans="1:29" ht="15.75" customHeight="1">
       <c r="N21" s="28"/>
     </row>
-    <row r="22" spans="1:28" ht="15.75" customHeight="1">
+    <row r="22" spans="1:29" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>123</v>
       </c>
@@ -3364,48 +3388,51 @@
       <c r="AB22" s="44" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="23" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC22" s="45" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="15.75" customHeight="1">
       <c r="A23" s="3">
         <v>0</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="66" t="s">
+      <c r="D23" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="66" t="s">
+      <c r="E23" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="55" t="s">
+      <c r="F23" s="52" t="s">
         <v>155</v>
       </c>
-      <c r="G23" s="54" t="s">
+      <c r="G23" s="51" t="s">
         <v>119</v>
       </c>
       <c r="H23" s="47" t="s">
         <v>176</v>
       </c>
-      <c r="I23" s="58" t="s">
+      <c r="I23" s="55" t="s">
         <v>190</v>
       </c>
-      <c r="J23" s="66" t="s">
+      <c r="J23" s="56" t="s">
         <v>64</v>
       </c>
       <c r="K23" s="47">
         <v>0</v>
       </c>
-      <c r="L23" s="50" t="s">
+      <c r="L23" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="M23" s="51" t="s">
+      <c r="M23" s="49" t="s">
         <v>227</v>
       </c>
-      <c r="N23" s="52" t="s">
+      <c r="N23" s="73" t="s">
         <v>238</v>
       </c>
       <c r="O23" s="46" t="s">
@@ -3450,24 +3477,27 @@
       <c r="AB23" s="46" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC23" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="15.75" customHeight="1">
       <c r="A24" s="3">
         <v>1</v>
       </c>
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="54"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="47"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="66"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="56"/>
       <c r="K24" s="47"/>
       <c r="L24" s="47"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="52"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="73"/>
       <c r="O24" s="47"/>
       <c r="P24" s="46"/>
       <c r="Q24" s="46"/>
@@ -3484,24 +3514,27 @@
       <c r="Z24" s="46"/>
       <c r="AA24" s="46"/>
       <c r="AB24" s="47"/>
-    </row>
-    <row r="25" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC24" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="15.75" customHeight="1">
       <c r="A25" s="3">
         <v>2</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="54"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="51"/>
       <c r="H25" s="47"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="66"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="56"/>
       <c r="K25" s="47"/>
       <c r="L25" s="47"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="52"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="73"/>
       <c r="O25" s="47"/>
       <c r="P25" s="46"/>
       <c r="Q25" s="46"/>
@@ -3516,24 +3549,27 @@
       <c r="Z25" s="46"/>
       <c r="AA25" s="46"/>
       <c r="AB25" s="47"/>
-    </row>
-    <row r="26" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC25" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="15.75" customHeight="1">
       <c r="A26" s="3">
         <v>3</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="54"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="51"/>
       <c r="H26" s="47"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="66"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="56"/>
       <c r="K26" s="47"/>
       <c r="L26" s="47"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="52"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="73"/>
       <c r="O26" s="47"/>
       <c r="P26" s="46"/>
       <c r="Q26" s="46"/>
@@ -3548,26 +3584,29 @@
       <c r="Z26" s="46"/>
       <c r="AA26" s="46"/>
       <c r="AB26" s="47"/>
-    </row>
-    <row r="27" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC26" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="15.75" customHeight="1">
       <c r="A27" s="3">
         <v>4</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54" t="s">
+      <c r="B27" s="51"/>
+      <c r="C27" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="54"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="51"/>
       <c r="H27" s="47"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="66"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="56"/>
       <c r="K27" s="47"/>
       <c r="L27" s="47"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="52"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="73"/>
       <c r="O27" s="47"/>
       <c r="P27" s="46"/>
       <c r="Q27" s="46"/>
@@ -3582,24 +3621,27 @@
       <c r="Z27" s="46"/>
       <c r="AA27" s="46"/>
       <c r="AB27" s="47"/>
-    </row>
-    <row r="28" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC27" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" ht="15.75" customHeight="1">
       <c r="A28" s="3">
         <v>5</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="54"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="51"/>
       <c r="H28" s="47"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="66"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="56"/>
       <c r="K28" s="47"/>
       <c r="L28" s="47"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="52"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="73"/>
       <c r="O28" s="47"/>
       <c r="P28" s="46"/>
       <c r="Q28" s="46"/>
@@ -3614,24 +3656,27 @@
       <c r="Z28" s="46"/>
       <c r="AA28" s="46"/>
       <c r="AB28" s="47"/>
-    </row>
-    <row r="29" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC28" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" ht="15.75" customHeight="1">
       <c r="A29" s="3">
         <v>6</v>
       </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="54"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="51"/>
       <c r="H29" s="47"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="66"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="56"/>
       <c r="K29" s="47"/>
       <c r="L29" s="47"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="52"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="73"/>
       <c r="O29" s="47"/>
       <c r="P29" s="46"/>
       <c r="Q29" s="46"/>
@@ -3648,36 +3693,39 @@
       <c r="Z29" s="46"/>
       <c r="AA29" s="46"/>
       <c r="AB29" s="47"/>
-    </row>
-    <row r="30" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC29" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" ht="15.75" customHeight="1">
       <c r="A30" s="3">
         <v>7</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54" t="s">
+      <c r="B30" s="51"/>
+      <c r="C30" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="D30" s="55" t="s">
+      <c r="D30" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="55" t="s">
+      <c r="E30" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="54" t="s">
+      <c r="F30" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="G30" s="54"/>
+      <c r="G30" s="51"/>
       <c r="H30" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="I30" s="58"/>
-      <c r="J30" s="55" t="s">
+      <c r="I30" s="55"/>
+      <c r="J30" s="52" t="s">
         <v>69</v>
       </c>
       <c r="K30" s="47"/>
       <c r="L30" s="47"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="52"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="73"/>
       <c r="O30" s="47">
         <v>2</v>
       </c>
@@ -3698,30 +3746,33 @@
       <c r="X30" s="46"/>
       <c r="Y30" s="46"/>
       <c r="Z30" s="46"/>
-      <c r="AA30" s="45" t="s">
+      <c r="AA30" s="48" t="s">
         <v>372</v>
       </c>
       <c r="AB30" s="46" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="31" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC30" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" ht="15.75" customHeight="1">
       <c r="A31" s="3">
         <v>8</v>
       </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
       <c r="H31" s="47"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="52"/>
       <c r="K31" s="47"/>
       <c r="L31" s="47"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="52"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="73"/>
       <c r="O31" s="47"/>
       <c r="P31" s="47"/>
       <c r="Q31" s="46"/>
@@ -3733,26 +3784,29 @@
       <c r="X31" s="46"/>
       <c r="Y31" s="46"/>
       <c r="Z31" s="46"/>
-      <c r="AA31" s="45"/>
+      <c r="AA31" s="48"/>
       <c r="AB31" s="47"/>
-    </row>
-    <row r="32" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC31" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" ht="15.75" customHeight="1">
       <c r="A32" s="3">
         <v>9</v>
       </c>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
       <c r="H32" s="47"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="52"/>
       <c r="K32" s="47"/>
       <c r="L32" s="47"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="52"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="73"/>
       <c r="O32" s="47"/>
       <c r="P32" s="47"/>
       <c r="Q32" s="46"/>
@@ -3768,36 +3822,39 @@
         <v>373</v>
       </c>
       <c r="AB32" s="47"/>
-    </row>
-    <row r="33" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC32" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" ht="15.75" customHeight="1">
       <c r="A33" s="3">
         <v>10</v>
       </c>
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="C33" s="64" t="s">
+      <c r="C33" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="D33" s="68" t="s">
+      <c r="D33" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="E33" s="68" t="s">
+      <c r="E33" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="54" t="s">
+      <c r="F33" s="51" t="s">
         <v>158</v>
       </c>
-      <c r="G33" s="69" t="s">
+      <c r="G33" s="67" t="s">
         <v>165</v>
       </c>
       <c r="H33" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="I33" s="58" t="s">
+      <c r="I33" s="55" t="s">
         <v>196</v>
       </c>
-      <c r="J33" s="68" t="s">
+      <c r="J33" s="57" t="s">
         <v>71</v>
       </c>
       <c r="K33" s="47"/>
@@ -3831,20 +3888,23 @@
       <c r="Z33" s="46"/>
       <c r="AA33" s="46"/>
       <c r="AB33" s="47"/>
-    </row>
-    <row r="34" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC33" s="45" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" ht="15.75" customHeight="1">
       <c r="A34" s="3">
         <v>11</v>
       </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="69"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="67"/>
       <c r="H34" s="47"/>
       <c r="I34" s="47"/>
-      <c r="J34" s="68"/>
+      <c r="J34" s="57"/>
       <c r="K34" s="47"/>
       <c r="L34" s="47"/>
       <c r="M34" s="46"/>
@@ -3864,13 +3924,16 @@
       <c r="Z34" s="46"/>
       <c r="AA34" s="46"/>
       <c r="AB34" s="47"/>
-    </row>
-    <row r="35" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC34" s="45" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" ht="15.75" customHeight="1">
       <c r="A35" s="3">
         <v>12</v>
       </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="51"/>
       <c r="D35" s="4" t="s">
         <v>144</v>
       </c>
@@ -3880,7 +3943,7 @@
       <c r="F35" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="G35" s="69"/>
+      <c r="G35" s="67"/>
       <c r="H35" s="3" t="s">
         <v>179</v>
       </c>
@@ -3889,7 +3952,7 @@
         <v>144</v>
       </c>
       <c r="K35" s="47"/>
-      <c r="L35" s="50" t="s">
+      <c r="L35" s="60" t="s">
         <v>191</v>
       </c>
       <c r="M35" s="46"/>
@@ -3919,36 +3982,39 @@
         <v>374</v>
       </c>
       <c r="AB35" s="47"/>
-    </row>
-    <row r="36" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC35" s="45" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" ht="15.75" customHeight="1">
       <c r="A36" s="3">
         <v>13</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="64" t="s">
+      <c r="C36" s="68" t="s">
         <v>142</v>
       </c>
-      <c r="D36" s="54" t="s">
+      <c r="D36" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="54" t="s">
+      <c r="E36" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="F36" s="54" t="s">
+      <c r="F36" s="51" t="s">
         <v>160</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="I36" s="59" t="s">
+      <c r="I36" s="72" t="s">
         <v>191</v>
       </c>
-      <c r="J36" s="54" t="s">
+      <c r="J36" s="51" t="s">
         <v>78</v>
       </c>
       <c r="K36" s="47"/>
@@ -3994,24 +4060,27 @@
       <c r="AB36" s="46" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="37" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC36" s="45" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" ht="15.75" customHeight="1">
       <c r="A37" s="3">
         <v>14</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="64"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
       <c r="G37" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="H37" s="48"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="54"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="51"/>
       <c r="K37" s="47">
         <v>1</v>
       </c>
@@ -4039,34 +4108,37 @@
       <c r="Z37" s="46"/>
       <c r="AA37" s="46"/>
       <c r="AB37" s="47"/>
-    </row>
-    <row r="38" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC37" s="45" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" ht="15.75" customHeight="1">
       <c r="A38" s="3">
         <v>15</v>
       </c>
-      <c r="B38" s="55" t="s">
+      <c r="B38" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="C38" s="55" t="s">
+      <c r="C38" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="54" t="s">
+      <c r="D38" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="E38" s="54" t="s">
+      <c r="E38" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="F38" s="54"/>
-      <c r="G38" s="69" t="s">
+      <c r="F38" s="51"/>
+      <c r="G38" s="67" t="s">
         <v>163</v>
       </c>
-      <c r="H38" s="48" t="s">
+      <c r="H38" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="I38" s="59" t="s">
+      <c r="I38" s="72" t="s">
         <v>192</v>
       </c>
-      <c r="J38" s="54" t="s">
+      <c r="J38" s="51" t="s">
         <v>83</v>
       </c>
       <c r="K38" s="47"/>
@@ -4074,7 +4146,7 @@
       <c r="M38" s="46" t="s">
         <v>231</v>
       </c>
-      <c r="N38" s="48" t="s">
+      <c r="N38" s="50" t="s">
         <v>242</v>
       </c>
       <c r="O38" s="47">
@@ -4100,28 +4172,31 @@
       <c r="AB38" s="46" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="39" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC38" s="45" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" ht="15.75" customHeight="1">
       <c r="A39" s="3">
         <v>16</v>
       </c>
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
       <c r="F39" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G39" s="69"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="54"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="51"/>
       <c r="K39" s="47"/>
       <c r="L39" s="46" t="s">
         <v>213</v>
       </c>
       <c r="M39" s="47"/>
-      <c r="N39" s="48"/>
+      <c r="N39" s="50"/>
       <c r="O39" s="47"/>
       <c r="P39" s="47"/>
       <c r="Q39" s="46" t="s">
@@ -4149,36 +4224,39 @@
         <v>376</v>
       </c>
       <c r="AB39" s="47"/>
-    </row>
-    <row r="40" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC39" s="45" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" ht="15.75" customHeight="1">
       <c r="A40" s="3">
         <v>17</v>
       </c>
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="64" t="s">
+      <c r="C40" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="D40" s="54" t="s">
+      <c r="D40" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="E40" s="54" t="s">
+      <c r="E40" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="F40" s="54" t="s">
+      <c r="F40" s="51" t="s">
         <v>162</v>
       </c>
-      <c r="G40" s="54" t="s">
+      <c r="G40" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="H40" s="48" t="s">
+      <c r="H40" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="I40" s="59" t="s">
+      <c r="I40" s="72" t="s">
         <v>194</v>
       </c>
-      <c r="J40" s="54" t="s">
+      <c r="J40" s="51" t="s">
         <v>87</v>
       </c>
       <c r="K40" s="47"/>
@@ -4189,7 +4267,7 @@
       <c r="N40" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="O40" s="52" t="s">
+      <c r="O40" s="73" t="s">
         <v>251</v>
       </c>
       <c r="P40" s="47"/>
@@ -4220,27 +4298,30 @@
       <c r="AB40" s="46" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="41" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC40" s="45" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" ht="15.75" customHeight="1">
       <c r="A41" s="3">
         <v>18</v>
       </c>
-      <c r="B41" s="54"/>
-      <c r="C41" s="54"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="54"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="54"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="72"/>
+      <c r="J41" s="51"/>
       <c r="K41" s="47"/>
       <c r="L41" s="47"/>
       <c r="M41" s="46"/>
-      <c r="N41" s="52" t="s">
+      <c r="N41" s="73" t="s">
         <v>245</v>
       </c>
-      <c r="O41" s="52"/>
+      <c r="O41" s="73"/>
       <c r="P41" s="47"/>
       <c r="Q41" s="46"/>
       <c r="R41" s="46" t="s">
@@ -4255,27 +4336,30 @@
       <c r="Z41" s="46"/>
       <c r="AA41" s="47"/>
       <c r="AB41" s="47"/>
-    </row>
-    <row r="42" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC41" s="45" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" ht="15.75" customHeight="1">
       <c r="A42" s="3">
         <v>19</v>
       </c>
-      <c r="B42" s="54"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="58" t="s">
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="55" t="s">
         <v>195</v>
       </c>
-      <c r="J42" s="54"/>
+      <c r="J42" s="51"/>
       <c r="K42" s="47"/>
       <c r="L42" s="47"/>
       <c r="M42" s="46"/>
-      <c r="N42" s="52"/>
-      <c r="O42" s="52"/>
+      <c r="N42" s="73"/>
+      <c r="O42" s="73"/>
       <c r="P42" s="47"/>
       <c r="Q42" s="46" t="s">
         <v>238</v>
@@ -4290,31 +4374,34 @@
       <c r="Z42" s="46"/>
       <c r="AA42" s="47"/>
       <c r="AB42" s="47"/>
-    </row>
-    <row r="43" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC42" s="45" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" ht="15.75" customHeight="1">
       <c r="A43" s="3">
         <v>20</v>
       </c>
-      <c r="B43" s="54"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="55" t="s">
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="I43" s="58"/>
-      <c r="J43" s="54"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="51"/>
       <c r="K43" s="47"/>
       <c r="L43" s="47"/>
       <c r="M43" s="46"/>
-      <c r="N43" s="53" t="s">
+      <c r="N43" s="74" t="s">
         <v>246</v>
       </c>
-      <c r="O43" s="52"/>
+      <c r="O43" s="73"/>
       <c r="P43" s="47"/>
       <c r="Q43" s="46"/>
       <c r="R43" s="47"/>
@@ -4327,25 +4414,28 @@
       <c r="Z43" s="46"/>
       <c r="AA43" s="47"/>
       <c r="AB43" s="47"/>
-    </row>
-    <row r="44" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC43" s="45" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" ht="15.75" customHeight="1">
       <c r="A44" s="3">
         <v>21</v>
       </c>
-      <c r="B44" s="54"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="54"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="51"/>
       <c r="K44" s="47"/>
       <c r="L44" s="47"/>
       <c r="M44" s="46"/>
-      <c r="N44" s="53"/>
-      <c r="O44" s="52"/>
+      <c r="N44" s="74"/>
+      <c r="O44" s="73"/>
       <c r="P44" s="47"/>
       <c r="Q44" s="46"/>
       <c r="R44" s="47"/>
@@ -4358,25 +4448,28 @@
       <c r="Z44" s="46"/>
       <c r="AA44" s="47"/>
       <c r="AB44" s="47"/>
-    </row>
-    <row r="45" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC44" s="45" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" ht="15.75" customHeight="1">
       <c r="A45" s="3">
         <v>22</v>
       </c>
-      <c r="B45" s="54"/>
-      <c r="C45" s="54"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="54"/>
-      <c r="F45" s="54"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="54"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="51"/>
       <c r="K45" s="47"/>
       <c r="L45" s="47"/>
       <c r="M45" s="46"/>
-      <c r="N45" s="53"/>
-      <c r="O45" s="52"/>
+      <c r="N45" s="74"/>
+      <c r="O45" s="73"/>
       <c r="P45" s="47"/>
       <c r="Q45" s="46"/>
       <c r="R45" s="47"/>
@@ -4389,27 +4482,30 @@
       <c r="Z45" s="46"/>
       <c r="AA45" s="47"/>
       <c r="AB45" s="47"/>
-    </row>
-    <row r="46" spans="1:28" ht="15.75" customHeight="1">
+      <c r="AC45" s="45" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" ht="15.75" customHeight="1">
       <c r="Q46" s="28"/>
     </row>
-    <row r="47" spans="1:28" ht="15.75" customHeight="1">
+    <row r="47" spans="1:29" ht="15.75" customHeight="1">
       <c r="Q47" s="28"/>
     </row>
-    <row r="48" spans="1:28" ht="15.75" customHeight="1">
+    <row r="48" spans="1:29" ht="15.75" customHeight="1">
       <c r="Q48" s="28"/>
     </row>
-    <row r="49" spans="1:33" ht="15.75" customHeight="1">
+    <row r="49" spans="1:34" ht="15.75" customHeight="1">
       <c r="Q49" s="28"/>
     </row>
-    <row r="50" spans="1:33" ht="15.75" customHeight="1">
+    <row r="50" spans="1:34" ht="15.75" customHeight="1">
       <c r="Q50" s="28"/>
     </row>
-    <row r="51" spans="1:33" ht="15.75" customHeight="1">
+    <row r="51" spans="1:34" ht="15.75" customHeight="1">
       <c r="Q51" s="28"/>
     </row>
-    <row r="52" spans="1:33" ht="15.75" customHeight="1"/>
-    <row r="53" spans="1:33" ht="15.75" customHeight="1">
+    <row r="52" spans="1:34" ht="15.75" customHeight="1"/>
+    <row r="53" spans="1:34" ht="15.75" customHeight="1">
       <c r="A53" s="8" t="s">
         <v>185</v>
       </c>
@@ -4509,63 +4605,66 @@
       <c r="AG53" s="44" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="54" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH53" s="45" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="54" spans="1:34" ht="15.75" customHeight="1">
       <c r="A54" s="8">
         <v>0</v>
       </c>
-      <c r="B54" s="61" t="s">
+      <c r="B54" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="C54" s="57" t="s">
+      <c r="C54" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="D54" s="57" t="s">
+      <c r="D54" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="E54" s="67" t="s">
+      <c r="E54" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="F54" s="57" t="s">
+      <c r="F54" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="G54" s="57" t="s">
+      <c r="G54" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="H54" s="61" t="s">
+      <c r="H54" s="66" t="s">
         <v>155</v>
       </c>
-      <c r="I54" s="57" t="s">
+      <c r="I54" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="J54" s="57" t="s">
+      <c r="J54" s="63" t="s">
         <v>172</v>
       </c>
-      <c r="K54" s="71" t="s">
+      <c r="K54" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="L54" s="60">
+      <c r="L54" s="59">
         <v>6</v>
       </c>
-      <c r="M54" s="60" t="s">
+      <c r="M54" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="N54" s="49" t="s">
+      <c r="N54" s="54" t="s">
         <v>200</v>
       </c>
       <c r="O54" s="47">
         <v>0</v>
       </c>
-      <c r="P54" s="50" t="s">
+      <c r="P54" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="Q54" s="49" t="s">
+      <c r="Q54" s="54" t="s">
         <v>200</v>
       </c>
       <c r="R54" s="46" t="s">
         <v>224</v>
       </c>
-      <c r="S54" s="51" t="s">
+      <c r="S54" s="49" t="s">
         <v>233</v>
       </c>
       <c r="T54" s="46" t="s">
@@ -4610,29 +4709,32 @@
       <c r="AG54" s="46" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="55" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH54" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="55" spans="1:34" ht="15.75" customHeight="1">
       <c r="A55" s="8">
         <v>1</v>
       </c>
-      <c r="B55" s="61"/>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="67"/>
-      <c r="F55" s="57"/>
-      <c r="G55" s="57"/>
-      <c r="H55" s="61"/>
-      <c r="I55" s="57"/>
-      <c r="J55" s="57"/>
-      <c r="K55" s="71"/>
-      <c r="L55" s="60"/>
-      <c r="M55" s="60"/>
+      <c r="B55" s="66"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="63"/>
+      <c r="E55" s="70"/>
+      <c r="F55" s="63"/>
+      <c r="G55" s="63"/>
+      <c r="H55" s="66"/>
+      <c r="I55" s="63"/>
+      <c r="J55" s="63"/>
+      <c r="K55" s="61"/>
+      <c r="L55" s="59"/>
+      <c r="M55" s="59"/>
       <c r="N55" s="47"/>
       <c r="O55" s="47"/>
       <c r="P55" s="47"/>
       <c r="Q55" s="47"/>
       <c r="R55" s="47"/>
-      <c r="S55" s="48"/>
+      <c r="S55" s="50"/>
       <c r="T55" s="47"/>
       <c r="U55" s="47"/>
       <c r="V55" s="47"/>
@@ -4651,29 +4753,32 @@
       <c r="AE55" s="46"/>
       <c r="AF55" s="46"/>
       <c r="AG55" s="47"/>
-    </row>
-    <row r="56" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH55" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="56" spans="1:34" ht="15.75" customHeight="1">
       <c r="A56" s="8">
         <v>2</v>
       </c>
-      <c r="B56" s="61"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="57"/>
-      <c r="E56" s="67"/>
-      <c r="F56" s="57"/>
-      <c r="G56" s="57"/>
-      <c r="H56" s="61"/>
-      <c r="I56" s="57"/>
-      <c r="J56" s="57"/>
-      <c r="K56" s="71"/>
-      <c r="L56" s="60"/>
-      <c r="M56" s="60"/>
+      <c r="B56" s="66"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="63"/>
+      <c r="E56" s="70"/>
+      <c r="F56" s="63"/>
+      <c r="G56" s="63"/>
+      <c r="H56" s="66"/>
+      <c r="I56" s="63"/>
+      <c r="J56" s="63"/>
+      <c r="K56" s="61"/>
+      <c r="L56" s="59"/>
+      <c r="M56" s="59"/>
       <c r="N56" s="47"/>
       <c r="O56" s="47"/>
       <c r="P56" s="47"/>
       <c r="Q56" s="47"/>
       <c r="R56" s="47"/>
-      <c r="S56" s="48"/>
+      <c r="S56" s="50"/>
       <c r="T56" s="47"/>
       <c r="U56" s="47"/>
       <c r="V56" s="47"/>
@@ -4688,29 +4793,32 @@
       <c r="AE56" s="46"/>
       <c r="AF56" s="46"/>
       <c r="AG56" s="47"/>
-    </row>
-    <row r="57" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH56" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="1:34" ht="15.75" customHeight="1">
       <c r="A57" s="8">
         <v>3</v>
       </c>
-      <c r="B57" s="61"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="67"/>
-      <c r="F57" s="57"/>
-      <c r="G57" s="57"/>
-      <c r="H57" s="61"/>
-      <c r="I57" s="57"/>
-      <c r="J57" s="57"/>
-      <c r="K57" s="71"/>
-      <c r="L57" s="60"/>
-      <c r="M57" s="60"/>
+      <c r="B57" s="66"/>
+      <c r="C57" s="63"/>
+      <c r="D57" s="63"/>
+      <c r="E57" s="70"/>
+      <c r="F57" s="63"/>
+      <c r="G57" s="63"/>
+      <c r="H57" s="66"/>
+      <c r="I57" s="63"/>
+      <c r="J57" s="63"/>
+      <c r="K57" s="61"/>
+      <c r="L57" s="59"/>
+      <c r="M57" s="59"/>
       <c r="N57" s="47"/>
       <c r="O57" s="47"/>
       <c r="P57" s="47"/>
       <c r="Q57" s="47"/>
       <c r="R57" s="47"/>
-      <c r="S57" s="48"/>
+      <c r="S57" s="50"/>
       <c r="T57" s="47"/>
       <c r="U57" s="47"/>
       <c r="V57" s="47"/>
@@ -4725,29 +4833,32 @@
       <c r="AE57" s="46"/>
       <c r="AF57" s="46"/>
       <c r="AG57" s="47"/>
-    </row>
-    <row r="58" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH57" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="58" spans="1:34" ht="15.75" customHeight="1">
       <c r="A58" s="8">
         <v>4</v>
       </c>
-      <c r="B58" s="61"/>
-      <c r="C58" s="57"/>
-      <c r="D58" s="57"/>
-      <c r="E58" s="67"/>
-      <c r="F58" s="57"/>
-      <c r="G58" s="57"/>
-      <c r="H58" s="61"/>
-      <c r="I58" s="57"/>
-      <c r="J58" s="57"/>
-      <c r="K58" s="71"/>
-      <c r="L58" s="60"/>
-      <c r="M58" s="60"/>
+      <c r="B58" s="66"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="70"/>
+      <c r="F58" s="63"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="66"/>
+      <c r="I58" s="63"/>
+      <c r="J58" s="63"/>
+      <c r="K58" s="61"/>
+      <c r="L58" s="59"/>
+      <c r="M58" s="59"/>
       <c r="N58" s="47"/>
       <c r="O58" s="47"/>
       <c r="P58" s="47"/>
       <c r="Q58" s="47"/>
       <c r="R58" s="47"/>
-      <c r="S58" s="48"/>
+      <c r="S58" s="50"/>
       <c r="T58" s="47"/>
       <c r="U58" s="47"/>
       <c r="V58" s="47"/>
@@ -4762,29 +4873,32 @@
       <c r="AE58" s="46"/>
       <c r="AF58" s="46"/>
       <c r="AG58" s="47"/>
-    </row>
-    <row r="59" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH58" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="59" spans="1:34" ht="15.75" customHeight="1">
       <c r="A59" s="8">
         <v>5</v>
       </c>
-      <c r="B59" s="61"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="57"/>
-      <c r="E59" s="67"/>
-      <c r="F59" s="57"/>
-      <c r="G59" s="57"/>
-      <c r="H59" s="61"/>
-      <c r="I59" s="57"/>
-      <c r="J59" s="57"/>
-      <c r="K59" s="71"/>
-      <c r="L59" s="60"/>
-      <c r="M59" s="60"/>
+      <c r="B59" s="66"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="70"/>
+      <c r="F59" s="63"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="66"/>
+      <c r="I59" s="63"/>
+      <c r="J59" s="63"/>
+      <c r="K59" s="61"/>
+      <c r="L59" s="59"/>
+      <c r="M59" s="59"/>
       <c r="N59" s="47"/>
       <c r="O59" s="47"/>
       <c r="P59" s="47"/>
       <c r="Q59" s="47"/>
       <c r="R59" s="47"/>
-      <c r="S59" s="48"/>
+      <c r="S59" s="50"/>
       <c r="T59" s="47"/>
       <c r="U59" s="47"/>
       <c r="V59" s="47"/>
@@ -4799,29 +4913,32 @@
       <c r="AE59" s="46"/>
       <c r="AF59" s="46"/>
       <c r="AG59" s="47"/>
-    </row>
-    <row r="60" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH59" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="60" spans="1:34" ht="15.75" customHeight="1">
       <c r="A60" s="8">
         <v>6</v>
       </c>
-      <c r="B60" s="61"/>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="67"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="57"/>
-      <c r="H60" s="61"/>
-      <c r="I60" s="57"/>
-      <c r="J60" s="57"/>
-      <c r="K60" s="71"/>
-      <c r="L60" s="60"/>
-      <c r="M60" s="60"/>
+      <c r="B60" s="66"/>
+      <c r="C60" s="63"/>
+      <c r="D60" s="63"/>
+      <c r="E60" s="70"/>
+      <c r="F60" s="63"/>
+      <c r="G60" s="63"/>
+      <c r="H60" s="66"/>
+      <c r="I60" s="63"/>
+      <c r="J60" s="63"/>
+      <c r="K60" s="61"/>
+      <c r="L60" s="59"/>
+      <c r="M60" s="59"/>
       <c r="N60" s="47"/>
       <c r="O60" s="47"/>
       <c r="P60" s="47"/>
       <c r="Q60" s="47"/>
       <c r="R60" s="47"/>
-      <c r="S60" s="48"/>
+      <c r="S60" s="50"/>
       <c r="T60" s="47"/>
       <c r="U60" s="47"/>
       <c r="V60" s="47"/>
@@ -4838,43 +4955,46 @@
       <c r="AE60" s="46"/>
       <c r="AF60" s="46"/>
       <c r="AG60" s="47"/>
-    </row>
-    <row r="61" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH60" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" spans="1:34" ht="15.75" customHeight="1">
       <c r="A61" s="8">
         <v>7</v>
       </c>
-      <c r="B61" s="61"/>
-      <c r="C61" s="57"/>
-      <c r="D61" s="57"/>
-      <c r="E61" s="56" t="s">
+      <c r="B61" s="66"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="F61" s="57"/>
-      <c r="G61" s="56" t="s">
+      <c r="F61" s="63"/>
+      <c r="G61" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="H61" s="62" t="s">
+      <c r="H61" s="65" t="s">
         <v>157</v>
       </c>
-      <c r="I61" s="57"/>
-      <c r="J61" s="57"/>
-      <c r="K61" s="71" t="s">
+      <c r="I61" s="63"/>
+      <c r="J61" s="63"/>
+      <c r="K61" s="61" t="s">
         <v>177</v>
       </c>
-      <c r="L61" s="60">
+      <c r="L61" s="59">
         <v>8</v>
       </c>
-      <c r="M61" s="60"/>
-      <c r="N61" s="49" t="s">
+      <c r="M61" s="59"/>
+      <c r="N61" s="54" t="s">
         <v>206</v>
       </c>
       <c r="O61" s="47"/>
       <c r="P61" s="47"/>
-      <c r="Q61" s="49" t="s">
+      <c r="Q61" s="54" t="s">
         <v>206</v>
       </c>
       <c r="R61" s="47"/>
-      <c r="S61" s="48"/>
+      <c r="S61" s="50"/>
       <c r="T61" s="47"/>
       <c r="U61" s="47">
         <v>2</v>
@@ -4889,35 +5009,38 @@
       <c r="AC61" s="46"/>
       <c r="AD61" s="46"/>
       <c r="AE61" s="46"/>
-      <c r="AF61" s="45" t="s">
+      <c r="AF61" s="48" t="s">
         <v>372</v>
       </c>
       <c r="AG61" s="46" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="62" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH61" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="62" spans="1:34" ht="15.75" customHeight="1">
       <c r="A62" s="8">
         <v>8</v>
       </c>
-      <c r="B62" s="61"/>
-      <c r="C62" s="57"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="57"/>
-      <c r="G62" s="56"/>
-      <c r="H62" s="62"/>
-      <c r="I62" s="57"/>
-      <c r="J62" s="57"/>
-      <c r="K62" s="71"/>
-      <c r="L62" s="60"/>
-      <c r="M62" s="60"/>
+      <c r="B62" s="66"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="63"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="63"/>
+      <c r="G62" s="53"/>
+      <c r="H62" s="65"/>
+      <c r="I62" s="63"/>
+      <c r="J62" s="63"/>
+      <c r="K62" s="61"/>
+      <c r="L62" s="59"/>
+      <c r="M62" s="59"/>
       <c r="N62" s="47"/>
       <c r="O62" s="47"/>
       <c r="P62" s="47"/>
       <c r="Q62" s="47"/>
       <c r="R62" s="47"/>
-      <c r="S62" s="48"/>
+      <c r="S62" s="50"/>
       <c r="T62" s="47"/>
       <c r="U62" s="47"/>
       <c r="V62" s="47"/>
@@ -4930,49 +5053,52 @@
       <c r="AC62" s="46"/>
       <c r="AD62" s="46"/>
       <c r="AE62" s="46"/>
-      <c r="AF62" s="45"/>
+      <c r="AF62" s="48"/>
       <c r="AG62" s="47"/>
-    </row>
-    <row r="63" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH62" s="45" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:34" ht="15.75" customHeight="1">
       <c r="A63" s="8">
         <v>9</v>
       </c>
-      <c r="B63" s="56" t="s">
+      <c r="B63" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="C63" s="62" t="s">
+      <c r="C63" s="65" t="s">
         <v>137</v>
       </c>
-      <c r="D63" s="62" t="s">
+      <c r="D63" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="E63" s="56"/>
-      <c r="F63" s="70" t="s">
+      <c r="E63" s="53"/>
+      <c r="F63" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="G63" s="56"/>
-      <c r="H63" s="62"/>
-      <c r="I63" s="56" t="s">
+      <c r="G63" s="53"/>
+      <c r="H63" s="65"/>
+      <c r="I63" s="53" t="s">
         <v>165</v>
       </c>
-      <c r="J63" s="56" t="s">
+      <c r="J63" s="53" t="s">
         <v>168</v>
       </c>
-      <c r="K63" s="72" t="s">
+      <c r="K63" s="62" t="s">
         <v>178</v>
       </c>
-      <c r="L63" s="60">
+      <c r="L63" s="59">
         <v>12</v>
       </c>
-      <c r="M63" s="60" t="s">
+      <c r="M63" s="59" t="s">
         <v>193</v>
       </c>
-      <c r="N63" s="49" t="s">
+      <c r="N63" s="54" t="s">
         <v>202</v>
       </c>
       <c r="O63" s="47"/>
       <c r="P63" s="47"/>
-      <c r="Q63" s="49" t="s">
+      <c r="Q63" s="54" t="s">
         <v>202</v>
       </c>
       <c r="R63" s="47"/>
@@ -4987,7 +5113,7 @@
       </c>
       <c r="V63" s="47"/>
       <c r="W63" s="46"/>
-      <c r="X63" s="45" t="s">
+      <c r="X63" s="48" t="s">
         <v>302</v>
       </c>
       <c r="Y63" s="47"/>
@@ -5003,27 +5129,30 @@
         <v>373</v>
       </c>
       <c r="AG63" s="47"/>
-    </row>
-    <row r="64" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH63" s="45" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="64" spans="1:34" ht="15.75" customHeight="1">
       <c r="A64" s="8">
         <v>10</v>
       </c>
-      <c r="B64" s="56"/>
-      <c r="C64" s="62"/>
-      <c r="D64" s="62"/>
-      <c r="E64" s="65" t="s">
+      <c r="B64" s="53"/>
+      <c r="C64" s="65"/>
+      <c r="D64" s="65"/>
+      <c r="E64" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="F64" s="70"/>
-      <c r="G64" s="56"/>
-      <c r="H64" s="62" t="s">
+      <c r="F64" s="64"/>
+      <c r="G64" s="53"/>
+      <c r="H64" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="I64" s="56"/>
-      <c r="J64" s="56"/>
-      <c r="K64" s="72"/>
-      <c r="L64" s="60"/>
-      <c r="M64" s="60"/>
+      <c r="I64" s="53"/>
+      <c r="J64" s="53"/>
+      <c r="K64" s="62"/>
+      <c r="L64" s="59"/>
+      <c r="M64" s="59"/>
       <c r="N64" s="47"/>
       <c r="O64" s="47"/>
       <c r="P64" s="47"/>
@@ -5036,7 +5165,7 @@
         <v>285</v>
       </c>
       <c r="W64" s="46"/>
-      <c r="X64" s="45"/>
+      <c r="X64" s="48"/>
       <c r="Y64" s="47"/>
       <c r="Z64" s="47"/>
       <c r="AA64" s="47"/>
@@ -5046,23 +5175,26 @@
       <c r="AE64" s="46"/>
       <c r="AF64" s="46"/>
       <c r="AG64" s="47"/>
-    </row>
-    <row r="65" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH64" s="45" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="65" spans="1:34" ht="15.75" customHeight="1">
       <c r="A65" s="8">
         <v>11</v>
       </c>
-      <c r="B65" s="56"/>
-      <c r="C65" s="62"/>
-      <c r="D65" s="62"/>
-      <c r="E65" s="65"/>
-      <c r="F65" s="70"/>
-      <c r="G65" s="56"/>
-      <c r="H65" s="62"/>
-      <c r="I65" s="56"/>
-      <c r="J65" s="56"/>
-      <c r="K65" s="72"/>
-      <c r="L65" s="60"/>
-      <c r="M65" s="60"/>
+      <c r="B65" s="53"/>
+      <c r="C65" s="65"/>
+      <c r="D65" s="65"/>
+      <c r="E65" s="69"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="53"/>
+      <c r="H65" s="65"/>
+      <c r="I65" s="53"/>
+      <c r="J65" s="53"/>
+      <c r="K65" s="62"/>
+      <c r="L65" s="59"/>
+      <c r="M65" s="59"/>
       <c r="N65" s="47"/>
       <c r="O65" s="47"/>
       <c r="P65" s="47"/>
@@ -5075,7 +5207,7 @@
       <c r="U65" s="47"/>
       <c r="V65" s="47"/>
       <c r="W65" s="46"/>
-      <c r="X65" s="45"/>
+      <c r="X65" s="48"/>
       <c r="Y65" s="47"/>
       <c r="Z65" s="47"/>
       <c r="AA65" s="47"/>
@@ -5087,34 +5219,37 @@
       <c r="AE65" s="46"/>
       <c r="AF65" s="46"/>
       <c r="AG65" s="47"/>
-    </row>
-    <row r="66" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH65" s="45" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="66" spans="1:34" ht="15.75" customHeight="1">
       <c r="A66" s="8">
         <v>12</v>
       </c>
-      <c r="B66" s="56"/>
-      <c r="C66" s="62"/>
-      <c r="D66" s="62"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="65"/>
+      <c r="D66" s="65"/>
       <c r="E66" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="F66" s="70"/>
+      <c r="F66" s="64"/>
       <c r="G66" s="8" t="s">
         <v>105</v>
       </c>
       <c r="H66" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="I66" s="56"/>
-      <c r="J66" s="56"/>
+      <c r="I66" s="53"/>
+      <c r="J66" s="53"/>
       <c r="K66" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="L66" s="60"/>
-      <c r="M66" s="60"/>
+      <c r="L66" s="59"/>
+      <c r="M66" s="59"/>
       <c r="N66" s="47"/>
       <c r="O66" s="47"/>
-      <c r="P66" s="50" t="s">
+      <c r="P66" s="60" t="s">
         <v>191</v>
       </c>
       <c r="Q66" s="47"/>
@@ -5128,7 +5263,7 @@
       <c r="W66" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="X66" s="45"/>
+      <c r="X66" s="48"/>
       <c r="Y66" s="47"/>
       <c r="Z66" s="47"/>
       <c r="AA66" s="47"/>
@@ -5146,53 +5281,56 @@
         <v>374</v>
       </c>
       <c r="AG66" s="47"/>
-    </row>
-    <row r="67" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH66" s="45" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="67" spans="1:34" ht="15.75" customHeight="1">
       <c r="A67" s="8">
         <v>13</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C67" s="62" t="s">
+      <c r="C67" s="65" t="s">
         <v>138</v>
       </c>
-      <c r="D67" s="62" t="s">
+      <c r="D67" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="E67" s="62" t="s">
+      <c r="E67" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="F67" s="62" t="s">
+      <c r="F67" s="65" t="s">
         <v>152</v>
       </c>
-      <c r="G67" s="56" t="s">
+      <c r="G67" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="H67" s="62" t="s">
+      <c r="H67" s="65" t="s">
         <v>160</v>
       </c>
       <c r="I67" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="J67" s="56" t="s">
+      <c r="J67" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="K67" s="72" t="s">
+      <c r="K67" s="62" t="s">
         <v>181</v>
       </c>
-      <c r="L67" s="60">
+      <c r="L67" s="59">
         <v>16</v>
       </c>
-      <c r="M67" s="60" t="s">
+      <c r="M67" s="59" t="s">
         <v>197</v>
       </c>
-      <c r="N67" s="49" t="s">
+      <c r="N67" s="54" t="s">
         <v>207</v>
       </c>
       <c r="O67" s="47"/>
       <c r="P67" s="47"/>
-      <c r="Q67" s="49" t="s">
+      <c r="Q67" s="54" t="s">
         <v>203</v>
       </c>
       <c r="R67" s="46" t="s">
@@ -5241,27 +5379,30 @@
       <c r="AG67" s="46" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="68" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH67" s="45" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="68" spans="1:34" ht="15.75" customHeight="1">
       <c r="A68" s="8">
         <v>14</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C68" s="62"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="62"/>
-      <c r="F68" s="62"/>
-      <c r="G68" s="56"/>
-      <c r="H68" s="62"/>
+      <c r="C68" s="65"/>
+      <c r="D68" s="65"/>
+      <c r="E68" s="65"/>
+      <c r="F68" s="65"/>
+      <c r="G68" s="53"/>
+      <c r="H68" s="65"/>
       <c r="I68" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="J68" s="56"/>
-      <c r="K68" s="72"/>
-      <c r="L68" s="60"/>
-      <c r="M68" s="60"/>
+      <c r="J68" s="53"/>
+      <c r="K68" s="62"/>
+      <c r="L68" s="59"/>
+      <c r="M68" s="59"/>
       <c r="N68" s="47"/>
       <c r="O68" s="47">
         <v>1</v>
@@ -5290,41 +5431,44 @@
       <c r="AE68" s="46"/>
       <c r="AF68" s="46"/>
       <c r="AG68" s="47"/>
-    </row>
-    <row r="69" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH68" s="45" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="69" spans="1:34" ht="15.75" customHeight="1">
       <c r="A69" s="8">
         <v>15</v>
       </c>
-      <c r="B69" s="56" t="s">
+      <c r="B69" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="C69" s="62" t="s">
+      <c r="C69" s="65" t="s">
         <v>139</v>
       </c>
-      <c r="D69" s="62" t="s">
+      <c r="D69" s="65" t="s">
         <v>145</v>
       </c>
-      <c r="E69" s="62" t="s">
+      <c r="E69" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="F69" s="62" t="s">
+      <c r="F69" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="G69" s="56" t="s">
+      <c r="G69" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="H69" s="62"/>
-      <c r="I69" s="56" t="s">
+      <c r="H69" s="65"/>
+      <c r="I69" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="J69" s="56" t="s">
+      <c r="J69" s="53" t="s">
         <v>170</v>
       </c>
-      <c r="K69" s="72" t="s">
+      <c r="K69" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="L69" s="60"/>
-      <c r="M69" s="73" t="s">
+      <c r="L69" s="59"/>
+      <c r="M69" s="58" t="s">
         <v>192</v>
       </c>
       <c r="N69" s="47"/>
@@ -5338,7 +5482,7 @@
       <c r="T69" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="U69" s="48">
+      <c r="U69" s="50">
         <v>6</v>
       </c>
       <c r="V69" s="29" t="s">
@@ -5363,35 +5507,38 @@
       <c r="AG69" s="46" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="70" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH69" s="45" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="70" spans="1:34" ht="15.75" customHeight="1">
       <c r="A70" s="8">
         <v>16</v>
       </c>
-      <c r="B70" s="56"/>
-      <c r="C70" s="62"/>
-      <c r="D70" s="62"/>
-      <c r="E70" s="62"/>
-      <c r="F70" s="62"/>
-      <c r="G70" s="56"/>
+      <c r="B70" s="53"/>
+      <c r="C70" s="65"/>
+      <c r="D70" s="65"/>
+      <c r="E70" s="65"/>
+      <c r="F70" s="65"/>
+      <c r="G70" s="53"/>
       <c r="H70" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="I70" s="56"/>
-      <c r="J70" s="56"/>
-      <c r="K70" s="72"/>
-      <c r="L70" s="60"/>
-      <c r="M70" s="73"/>
+      <c r="I70" s="53"/>
+      <c r="J70" s="53"/>
+      <c r="K70" s="62"/>
+      <c r="L70" s="59"/>
+      <c r="M70" s="58"/>
       <c r="N70" s="47"/>
       <c r="O70" s="47"/>
-      <c r="P70" s="50" t="s">
+      <c r="P70" s="60" t="s">
         <v>213</v>
       </c>
       <c r="Q70" s="47"/>
       <c r="R70" s="47"/>
       <c r="S70" s="46"/>
       <c r="T70" s="47"/>
-      <c r="U70" s="48"/>
+      <c r="U70" s="50"/>
       <c r="V70" s="46" t="s">
         <v>286</v>
       </c>
@@ -5418,8 +5565,11 @@
         <v>376</v>
       </c>
       <c r="AG70" s="47"/>
-    </row>
-    <row r="71" spans="1:33" ht="15.75" customHeight="1">
+      <c r="AH70" s="45" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="71" spans="1:34" ht="15.75" customHeight="1">
       <c r="A71" s="8" t="s">
         <v>124</v>
       </c>
@@ -5463,7 +5613,7 @@
         <v>208</v>
       </c>
       <c r="O71" s="47"/>
-      <c r="P71" s="50"/>
+      <c r="P71" s="60"/>
       <c r="Q71" s="23" t="s">
         <v>208</v>
       </c>
@@ -5505,9 +5655,12 @@
       <c r="AG71" s="34" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="72" spans="1:33" ht="15.75" customHeight="1">
-      <c r="B72" s="54"/>
+      <c r="AH71" s="45" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="72" spans="1:34" ht="15.75" customHeight="1">
+      <c r="B72" s="51"/>
       <c r="K72" s="5"/>
       <c r="O72" s="22"/>
       <c r="P72" s="22"/>
@@ -5518,8 +5671,8 @@
       <c r="AE72" s="34"/>
       <c r="AG72" s="22"/>
     </row>
-    <row r="73" spans="1:33" ht="15.75" customHeight="1">
-      <c r="B73" s="54"/>
+    <row r="73" spans="1:34" ht="15.75" customHeight="1">
+      <c r="B73" s="51"/>
       <c r="K73" s="5"/>
       <c r="O73" s="22"/>
       <c r="P73" s="22"/>
@@ -5530,10 +5683,10 @@
       <c r="AE73" s="34"/>
       <c r="AG73" s="22"/>
     </row>
-    <row r="74" spans="1:33" ht="15.75" customHeight="1">
-      <c r="B74" s="54"/>
-      <c r="I74" s="55"/>
-      <c r="K74" s="48"/>
+    <row r="74" spans="1:34" ht="15.75" customHeight="1">
+      <c r="B74" s="51"/>
+      <c r="I74" s="52"/>
+      <c r="K74" s="50"/>
       <c r="O74" s="22"/>
       <c r="P74" s="22"/>
       <c r="X74" s="22"/>
@@ -5543,10 +5696,10 @@
       <c r="AE74" s="34"/>
       <c r="AG74" s="22"/>
     </row>
-    <row r="75" spans="1:33" ht="15.75" customHeight="1">
-      <c r="B75" s="54"/>
-      <c r="I75" s="55"/>
-      <c r="K75" s="48"/>
+    <row r="75" spans="1:34" ht="15.75" customHeight="1">
+      <c r="B75" s="51"/>
+      <c r="I75" s="52"/>
+      <c r="K75" s="50"/>
       <c r="O75" s="22"/>
       <c r="P75" s="22"/>
       <c r="X75" s="22"/>
@@ -5556,10 +5709,10 @@
       <c r="AE75" s="34"/>
       <c r="AG75" s="22"/>
     </row>
-    <row r="76" spans="1:33" ht="15.75" customHeight="1">
-      <c r="B76" s="54"/>
-      <c r="I76" s="55"/>
-      <c r="K76" s="48"/>
+    <row r="76" spans="1:34" ht="15.75" customHeight="1">
+      <c r="B76" s="51"/>
+      <c r="I76" s="52"/>
+      <c r="K76" s="50"/>
       <c r="O76" s="22"/>
       <c r="P76" s="22"/>
       <c r="X76" s="22"/>
@@ -5569,12 +5722,12 @@
       <c r="AE76" s="34"/>
       <c r="AG76" s="22"/>
     </row>
-    <row r="77" spans="1:33" ht="15.75" customHeight="1">
-      <c r="B77" s="54"/>
-    </row>
-    <row r="78" spans="1:33" ht="15.75" customHeight="1"/>
-    <row r="79" spans="1:33" ht="15.75" customHeight="1"/>
-    <row r="80" spans="1:33" ht="15.75" customHeight="1"/>
+    <row r="77" spans="1:34" ht="15.75" customHeight="1">
+      <c r="B77" s="51"/>
+    </row>
+    <row r="78" spans="1:34" ht="15.75" customHeight="1"/>
+    <row r="79" spans="1:34" ht="15.75" customHeight="1"/>
+    <row r="80" spans="1:34" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -6498,6 +6651,275 @@
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="293">
+    <mergeCell ref="AF61:AF62"/>
+    <mergeCell ref="AF54:AF60"/>
+    <mergeCell ref="AF63:AF65"/>
+    <mergeCell ref="AF67:AF69"/>
+    <mergeCell ref="AA23:AA29"/>
+    <mergeCell ref="AA30:AA31"/>
+    <mergeCell ref="AA32:AA34"/>
+    <mergeCell ref="AA36:AA38"/>
+    <mergeCell ref="AA40:AA45"/>
+    <mergeCell ref="AE54:AE65"/>
+    <mergeCell ref="AE67:AE69"/>
+    <mergeCell ref="AD67:AD71"/>
+    <mergeCell ref="AD55:AD64"/>
+    <mergeCell ref="X23:X35"/>
+    <mergeCell ref="X36:X38"/>
+    <mergeCell ref="X40:X45"/>
+    <mergeCell ref="AC54:AC66"/>
+    <mergeCell ref="AC67:AC69"/>
+    <mergeCell ref="Y36:Y45"/>
+    <mergeCell ref="Y24:Y33"/>
+    <mergeCell ref="AB23:AB29"/>
+    <mergeCell ref="AB30:AB35"/>
+    <mergeCell ref="S67:S68"/>
+    <mergeCell ref="S69:S71"/>
+    <mergeCell ref="T69:T70"/>
+    <mergeCell ref="U54:U60"/>
+    <mergeCell ref="U61:U62"/>
+    <mergeCell ref="U63:U66"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="U69:U70"/>
+    <mergeCell ref="R67:R71"/>
+    <mergeCell ref="O40:O45"/>
+    <mergeCell ref="T54:T62"/>
+    <mergeCell ref="T63:T66"/>
+    <mergeCell ref="Q61:Q62"/>
+    <mergeCell ref="Q63:Q66"/>
+    <mergeCell ref="Q67:Q70"/>
+    <mergeCell ref="O54:O67"/>
+    <mergeCell ref="P54:P65"/>
+    <mergeCell ref="P66:P69"/>
+    <mergeCell ref="O68:O71"/>
+    <mergeCell ref="P70:P71"/>
+    <mergeCell ref="M2:M11"/>
+    <mergeCell ref="M12:M18"/>
+    <mergeCell ref="M23:M32"/>
+    <mergeCell ref="M33:M35"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="M40:M45"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="N5:N11"/>
+    <mergeCell ref="N12:N18"/>
+    <mergeCell ref="O23:O29"/>
+    <mergeCell ref="O2:O11"/>
+    <mergeCell ref="O12:O18"/>
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="O33:O35"/>
+    <mergeCell ref="N54:N60"/>
+    <mergeCell ref="N61:N62"/>
+    <mergeCell ref="N63:N66"/>
+    <mergeCell ref="N33:N35"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="N23:N32"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="N43:N45"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="L12:L16"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="N67:N70"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="G61:G65"/>
+    <mergeCell ref="G54:G60"/>
+    <mergeCell ref="H23:H29"/>
+    <mergeCell ref="H30:H32"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="H40:H42"/>
+    <mergeCell ref="H43:H45"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="I42:I45"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="I23:I32"/>
+    <mergeCell ref="M54:M62"/>
+    <mergeCell ref="M63:M66"/>
+    <mergeCell ref="M67:M68"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B72:B77"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B23:B32"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B45"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="B54:B62"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C54:C62"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="E2:E11"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C45"/>
+    <mergeCell ref="E12:E18"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="E23:E29"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E54:E60"/>
+    <mergeCell ref="E61:E63"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="D54:D62"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D40:D45"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="E40:E45"/>
+    <mergeCell ref="D23:D29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="F23:F29"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="F40:F45"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="G23:G32"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="F54:F62"/>
+    <mergeCell ref="F63:F66"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="I74:I76"/>
+    <mergeCell ref="I54:I62"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="H54:H60"/>
+    <mergeCell ref="H61:H63"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="H67:H69"/>
+    <mergeCell ref="K74:K76"/>
+    <mergeCell ref="K61:K62"/>
+    <mergeCell ref="K63:K65"/>
+    <mergeCell ref="K54:K60"/>
+    <mergeCell ref="K67:K68"/>
+    <mergeCell ref="K69:K70"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="J63:J66"/>
+    <mergeCell ref="J69:J70"/>
+    <mergeCell ref="J54:J62"/>
+    <mergeCell ref="M69:M70"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="L54:L60"/>
+    <mergeCell ref="L61:L62"/>
+    <mergeCell ref="L63:L66"/>
+    <mergeCell ref="L67:L70"/>
+    <mergeCell ref="L23:L34"/>
+    <mergeCell ref="L35:L38"/>
+    <mergeCell ref="L39:L45"/>
+    <mergeCell ref="K12:K16"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="I2:I7"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="I69:I70"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="J23:J29"/>
+    <mergeCell ref="J30:J32"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="J40:J45"/>
+    <mergeCell ref="K23:K36"/>
+    <mergeCell ref="K37:K45"/>
+    <mergeCell ref="P2:P11"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="P14:P16"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="S54:S62"/>
+    <mergeCell ref="S63:S64"/>
+    <mergeCell ref="P23:P29"/>
+    <mergeCell ref="P36:P45"/>
+    <mergeCell ref="P33:P35"/>
+    <mergeCell ref="P30:P32"/>
+    <mergeCell ref="R23:R28"/>
+    <mergeCell ref="R29:R34"/>
+    <mergeCell ref="R38:R39"/>
+    <mergeCell ref="R41:R45"/>
+    <mergeCell ref="R36:R37"/>
+    <mergeCell ref="Q39:Q41"/>
+    <mergeCell ref="Q42:Q45"/>
+    <mergeCell ref="Q33:Q37"/>
+    <mergeCell ref="Q23:Q32"/>
+    <mergeCell ref="R54:R66"/>
+    <mergeCell ref="S23:S32"/>
+    <mergeCell ref="S33:S35"/>
+    <mergeCell ref="S40:S45"/>
+    <mergeCell ref="Q54:Q60"/>
+    <mergeCell ref="AB40:AB45"/>
+    <mergeCell ref="V54:V63"/>
+    <mergeCell ref="V64:V68"/>
+    <mergeCell ref="V70:V71"/>
+    <mergeCell ref="T23:T29"/>
+    <mergeCell ref="T30:T45"/>
+    <mergeCell ref="U23:U29"/>
+    <mergeCell ref="U30:U32"/>
+    <mergeCell ref="U40:U45"/>
+    <mergeCell ref="U36:U38"/>
+    <mergeCell ref="U33:U34"/>
+    <mergeCell ref="V23:V30"/>
+    <mergeCell ref="W23:W34"/>
+    <mergeCell ref="Z23:Z34"/>
+    <mergeCell ref="Z36:Z38"/>
+    <mergeCell ref="Z40:Z45"/>
     <mergeCell ref="AG54:AG60"/>
     <mergeCell ref="AG61:AG66"/>
     <mergeCell ref="AG67:AG68"/>
@@ -6522,275 +6944,6 @@
     <mergeCell ref="AA55:AA62"/>
     <mergeCell ref="AB36:AB37"/>
     <mergeCell ref="AB38:AB39"/>
-    <mergeCell ref="AB40:AB45"/>
-    <mergeCell ref="V54:V63"/>
-    <mergeCell ref="V64:V68"/>
-    <mergeCell ref="V70:V71"/>
-    <mergeCell ref="T23:T29"/>
-    <mergeCell ref="T30:T45"/>
-    <mergeCell ref="U23:U29"/>
-    <mergeCell ref="U30:U32"/>
-    <mergeCell ref="U40:U45"/>
-    <mergeCell ref="U36:U38"/>
-    <mergeCell ref="U33:U34"/>
-    <mergeCell ref="V23:V30"/>
-    <mergeCell ref="W23:W34"/>
-    <mergeCell ref="P2:P11"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="P14:P16"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="S54:S62"/>
-    <mergeCell ref="S63:S64"/>
-    <mergeCell ref="P23:P29"/>
-    <mergeCell ref="P36:P45"/>
-    <mergeCell ref="P33:P35"/>
-    <mergeCell ref="P30:P32"/>
-    <mergeCell ref="R23:R28"/>
-    <mergeCell ref="R29:R34"/>
-    <mergeCell ref="R38:R39"/>
-    <mergeCell ref="R41:R45"/>
-    <mergeCell ref="R36:R37"/>
-    <mergeCell ref="Q39:Q41"/>
-    <mergeCell ref="Q42:Q45"/>
-    <mergeCell ref="Q33:Q37"/>
-    <mergeCell ref="Q23:Q32"/>
-    <mergeCell ref="R54:R66"/>
-    <mergeCell ref="S23:S32"/>
-    <mergeCell ref="S33:S35"/>
-    <mergeCell ref="S40:S45"/>
-    <mergeCell ref="I2:I7"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="I69:I70"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="J23:J29"/>
-    <mergeCell ref="J30:J32"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="J40:J45"/>
-    <mergeCell ref="K23:K36"/>
-    <mergeCell ref="K37:K45"/>
-    <mergeCell ref="M69:M70"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="L54:L60"/>
-    <mergeCell ref="L61:L62"/>
-    <mergeCell ref="L63:L66"/>
-    <mergeCell ref="L67:L70"/>
-    <mergeCell ref="L23:L34"/>
-    <mergeCell ref="L35:L38"/>
-    <mergeCell ref="L39:L45"/>
-    <mergeCell ref="K74:K76"/>
-    <mergeCell ref="K61:K62"/>
-    <mergeCell ref="K63:K65"/>
-    <mergeCell ref="K54:K60"/>
-    <mergeCell ref="K67:K68"/>
-    <mergeCell ref="K69:K70"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="J63:J66"/>
-    <mergeCell ref="J69:J70"/>
-    <mergeCell ref="J54:J62"/>
-    <mergeCell ref="F54:F62"/>
-    <mergeCell ref="F63:F66"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="I74:I76"/>
-    <mergeCell ref="I54:I62"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="H54:H60"/>
-    <mergeCell ref="H61:H63"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="H67:H69"/>
-    <mergeCell ref="F23:F29"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="F40:F45"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="G23:G32"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="D54:D62"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D40:D45"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="E40:E45"/>
-    <mergeCell ref="D23:D29"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C45"/>
-    <mergeCell ref="E12:E18"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="E23:E29"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="E54:E60"/>
-    <mergeCell ref="E61:E63"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="E2:E11"/>
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B72:B77"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B23:B32"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B45"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="B54:B62"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="D2:D7"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C54:C62"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="N67:N70"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="G61:G65"/>
-    <mergeCell ref="G54:G60"/>
-    <mergeCell ref="H23:H29"/>
-    <mergeCell ref="H30:H32"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="H40:H42"/>
-    <mergeCell ref="H43:H45"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="I42:I45"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="I23:I32"/>
-    <mergeCell ref="M54:M62"/>
-    <mergeCell ref="M63:M66"/>
-    <mergeCell ref="M67:M68"/>
-    <mergeCell ref="K12:K16"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="N54:N60"/>
-    <mergeCell ref="N61:N62"/>
-    <mergeCell ref="N63:N66"/>
-    <mergeCell ref="N33:N35"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="N23:N32"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="N43:N45"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="L8:L11"/>
-    <mergeCell ref="L12:L16"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="Q54:Q60"/>
-    <mergeCell ref="Q61:Q62"/>
-    <mergeCell ref="Q63:Q66"/>
-    <mergeCell ref="Q67:Q70"/>
-    <mergeCell ref="O54:O67"/>
-    <mergeCell ref="P54:P65"/>
-    <mergeCell ref="P66:P69"/>
-    <mergeCell ref="O68:O71"/>
-    <mergeCell ref="P70:P71"/>
-    <mergeCell ref="M2:M11"/>
-    <mergeCell ref="M12:M18"/>
-    <mergeCell ref="M23:M32"/>
-    <mergeCell ref="M33:M35"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="M40:M45"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="N5:N11"/>
-    <mergeCell ref="N12:N18"/>
-    <mergeCell ref="O23:O29"/>
-    <mergeCell ref="O2:O11"/>
-    <mergeCell ref="O12:O18"/>
-    <mergeCell ref="S67:S68"/>
-    <mergeCell ref="S69:S71"/>
-    <mergeCell ref="T69:T70"/>
-    <mergeCell ref="U54:U60"/>
-    <mergeCell ref="U61:U62"/>
-    <mergeCell ref="U63:U66"/>
-    <mergeCell ref="O38:O39"/>
-    <mergeCell ref="U69:U70"/>
-    <mergeCell ref="R67:R71"/>
-    <mergeCell ref="O40:O45"/>
-    <mergeCell ref="O30:O32"/>
-    <mergeCell ref="O33:O35"/>
-    <mergeCell ref="T54:T62"/>
-    <mergeCell ref="T63:T66"/>
-    <mergeCell ref="Z23:Z34"/>
-    <mergeCell ref="Z36:Z38"/>
-    <mergeCell ref="Z40:Z45"/>
-    <mergeCell ref="AE54:AE65"/>
-    <mergeCell ref="AE67:AE69"/>
-    <mergeCell ref="AD67:AD71"/>
-    <mergeCell ref="AD55:AD64"/>
-    <mergeCell ref="X23:X35"/>
-    <mergeCell ref="X36:X38"/>
-    <mergeCell ref="X40:X45"/>
-    <mergeCell ref="AC54:AC66"/>
-    <mergeCell ref="AC67:AC69"/>
-    <mergeCell ref="Y36:Y45"/>
-    <mergeCell ref="Y24:Y33"/>
-    <mergeCell ref="AB23:AB29"/>
-    <mergeCell ref="AB30:AB35"/>
-    <mergeCell ref="AF61:AF62"/>
-    <mergeCell ref="AF54:AF60"/>
-    <mergeCell ref="AF63:AF65"/>
-    <mergeCell ref="AF67:AF69"/>
-    <mergeCell ref="AA23:AA29"/>
-    <mergeCell ref="AA30:AA31"/>
-    <mergeCell ref="AA32:AA34"/>
-    <mergeCell ref="AA36:AA38"/>
-    <mergeCell ref="AA40:AA45"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -6935,13 +7088,13 @@
       <c r="B6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="75" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="E6" s="74" t="s">
+      <c r="E6" s="75" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="43" t="s">
@@ -6958,11 +7111,11 @@
       <c r="B7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="75"/>
+      <c r="C7" s="76"/>
       <c r="D7" s="37" t="s">
         <v>315</v>
       </c>
-      <c r="E7" s="75"/>
+      <c r="E7" s="76"/>
       <c r="F7" s="43" t="s">
         <v>352</v>
       </c>
@@ -7107,7 +7260,7 @@
       <c r="A18" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="76" t="s">
         <v>267</v>
       </c>
       <c r="C18" s="31"/>
@@ -7118,7 +7271,7 @@
       <c r="A19" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="B19" s="75"/>
+      <c r="B19" s="76"/>
       <c r="C19" s="31"/>
       <c r="D19" s="32"/>
       <c r="G19" s="31"/>
@@ -7127,7 +7280,7 @@
       <c r="A20" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="B20" s="75"/>
+      <c r="B20" s="76"/>
       <c r="C20" s="31"/>
       <c r="D20" s="32"/>
       <c r="G20" s="31"/>
@@ -7136,7 +7289,7 @@
       <c r="A21" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="76" t="s">
         <v>268</v>
       </c>
       <c r="C21" s="31"/>
@@ -7147,7 +7300,7 @@
       <c r="A22" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="B22" s="75"/>
+      <c r="B22" s="76"/>
       <c r="C22" s="31"/>
       <c r="D22" s="32"/>
       <c r="G22" s="31"/>
@@ -7156,7 +7309,7 @@
       <c r="A23" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="B23" s="75"/>
+      <c r="B23" s="76"/>
       <c r="C23" s="31"/>
       <c r="D23" s="32"/>
       <c r="G23" s="31"/>
@@ -7165,7 +7318,7 @@
       <c r="A24" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="B24" s="75"/>
+      <c r="B24" s="76"/>
       <c r="C24" s="31"/>
       <c r="D24" s="32"/>
       <c r="G24" s="31"/>
@@ -7174,7 +7327,7 @@
       <c r="A25" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="B25" s="75"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="31"/>
       <c r="D25" s="32"/>
       <c r="G25" s="31"/>

</xml_diff>